<commit_message>
28.06 Excel integration: parsing cell's value storing rows and columns
</commit_message>
<xml_diff>
--- a/ExcelDriven/src/test/resources/workbook1.xlsx
+++ b/ExcelDriven/src/test/resources/workbook1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Testcases</t>
   </si>
@@ -39,49 +39,73 @@
     <t>Delete Profile</t>
   </si>
   <si>
-    <t>eweed</t>
-  </si>
-  <si>
-    <t>sdasda</t>
-  </si>
-  <si>
-    <t>sdasd</t>
-  </si>
-  <si>
-    <t>zxczxc</t>
-  </si>
-  <si>
-    <t>cxzxcz</t>
-  </si>
-  <si>
     <t>Ignore Profile</t>
   </si>
   <si>
-    <t>iuyiuy</t>
-  </si>
-  <si>
-    <t>iuyiyu</t>
-  </si>
-  <si>
-    <t>qweqw</t>
-  </si>
-  <si>
-    <t>qweq</t>
-  </si>
-  <si>
-    <t>hgfghf</t>
-  </si>
-  <si>
-    <t>hghgf</t>
-  </si>
-  <si>
     <t>Login test</t>
   </si>
   <si>
-    <t>fghghg</t>
-  </si>
-  <si>
-    <t>asdas</t>
+    <t>Data4</t>
+  </si>
+  <si>
+    <t>2-2</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>2-4</t>
+  </si>
+  <si>
+    <t>2-5</t>
+  </si>
+  <si>
+    <t>3-2</t>
+  </si>
+  <si>
+    <t>3-3</t>
+  </si>
+  <si>
+    <t>4-2</t>
+  </si>
+  <si>
+    <t>5-2</t>
+  </si>
+  <si>
+    <t>6-2</t>
+  </si>
+  <si>
+    <t>3-4</t>
+  </si>
+  <si>
+    <t>3-5</t>
+  </si>
+  <si>
+    <t>4-3</t>
+  </si>
+  <si>
+    <t>4-4</t>
+  </si>
+  <si>
+    <t>4-5</t>
+  </si>
+  <si>
+    <t>5-3</t>
+  </si>
+  <si>
+    <t>5-4</t>
+  </si>
+  <si>
+    <t>5-5</t>
+  </si>
+  <si>
+    <t>6-3</t>
+  </si>
+  <si>
+    <t>6-4</t>
+  </si>
+  <si>
+    <t>6-5</t>
   </si>
 </sst>
 </file>
@@ -118,8 +142,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -414,106 +439,126 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="E3" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" t="s">
-        <v>14</v>
+      <c r="C6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -522,7 +567,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="E6" sqref="A1:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>